<commit_message>
add shared ADC and caps
</commit_message>
<xml_diff>
--- a/model/RunControl.xlsx
+++ b/model/RunControl.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90669DD-22B6-448E-AB9F-AE89616971FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64558DA4-1C31-4A2A-86BD-305C6DE1F90E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1845" windowWidth="29040" windowHeight="15840" tabRatio="524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,7 +77,7 @@
     See tab "Note1" for explanations of the combinations of parameters "use_baselineUAAL" and "newBasisPolicyChg"</t>
       </text>
     </comment>
-    <comment ref="R4" authorId="2" shapeId="0" xr:uid="{CAF507CB-F634-4E84-8E7F-17CD8E2A0EDC}">
+    <comment ref="S4" authorId="2" shapeId="0" xr:uid="{CAF507CB-F634-4E84-8E7F-17CD8E2A0EDC}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -85,7 +85,7 @@
     the DR used in determining COLA. Leave blank (NA when loaded) if the DR for regular valuation is used.</t>
       </text>
     </comment>
-    <comment ref="W4" authorId="3" shapeId="0" xr:uid="{8515E407-C037-4E97-A4C6-62FC0108B1A6}">
+    <comment ref="X4" authorId="3" shapeId="0" xr:uid="{8515E407-C037-4E97-A4C6-62FC0108B1A6}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -93,7 +93,7 @@
     The esclator is calibrated from 2.75% to 3.5% to match the 2018 SC</t>
       </text>
     </comment>
-    <comment ref="AA4" authorId="0" shapeId="0" xr:uid="{568404F5-400A-46EF-8AA1-93D4C44E460E}">
+    <comment ref="AB4" authorId="0" shapeId="0" xr:uid="{568404F5-400A-46EF-8AA1-93D4C44E460E}">
       <text>
         <r>
           <rPr>
@@ -118,7 +118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK4" authorId="0" shapeId="0" xr:uid="{148CF5FB-6519-420B-97E2-DCE9E3F8AE4C}">
+    <comment ref="AL4" authorId="0" shapeId="0" xr:uid="{148CF5FB-6519-420B-97E2-DCE9E3F8AE4C}">
       <text>
         <r>
           <rPr>
@@ -235,7 +235,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="273">
   <si>
     <t>nsim</t>
   </si>
@@ -1111,6 +1111,12 @@
   </si>
   <si>
     <t>EEC_share</t>
+  </si>
+  <si>
+    <t>EEC_type</t>
+  </si>
+  <si>
+    <t>sharedADC</t>
   </si>
 </sst>
 </file>
@@ -1785,10 +1791,10 @@
   <threadedComment ref="H4" dT="2020-11-29T15:06:08.38" personId="{00000000-0000-0000-0000-000000000000}" id="{1E17415D-3C00-4D50-B13B-6BE374701D46}">
     <text>See tab "Note1" for explanations of the combinations of parameters "use_baselineUAAL" and "newBasisPolicyChg"</text>
   </threadedComment>
-  <threadedComment ref="R4" dT="2020-08-16T01:43:29.52" personId="{00000000-0000-0000-0000-000000000000}" id="{CAF507CB-F634-4E84-8E7F-17CD8E2A0EDC}">
+  <threadedComment ref="S4" dT="2020-08-16T01:43:29.52" personId="{00000000-0000-0000-0000-000000000000}" id="{CAF507CB-F634-4E84-8E7F-17CD8E2A0EDC}">
     <text>the DR used in determining COLA. Leave blank (NA when loaded) if the DR for regular valuation is used.</text>
   </threadedComment>
-  <threadedComment ref="W4" dT="2020-12-06T12:17:58.66" personId="{00000000-0000-0000-0000-000000000000}" id="{8515E407-C037-4E97-A4C6-62FC0108B1A6}">
+  <threadedComment ref="X4" dT="2020-12-06T12:17:58.66" personId="{00000000-0000-0000-0000-000000000000}" id="{8515E407-C037-4E97-A4C6-62FC0108B1A6}">
     <text>The esclator is calibrated from 2.75% to 3.5% to match the 2018 SC</text>
   </threadedComment>
 </ThreadedComments>
@@ -1823,13 +1829,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D014B46A-D012-4D18-AEAB-1D829080B2CE}">
-  <dimension ref="A2:AW9"/>
+  <dimension ref="A2:AX9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="4" topLeftCell="J5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="N19" sqref="N19"/>
+      <selection pane="bottomRight" activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1845,42 +1851,43 @@
     <col min="9" max="9" width="19.7109375" customWidth="1"/>
     <col min="10" max="10" width="16.85546875" customWidth="1"/>
     <col min="11" max="14" width="12.5703125" customWidth="1"/>
-    <col min="15" max="15" width="17.7109375" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.85546875" customWidth="1"/>
-    <col min="19" max="19" width="25.85546875" customWidth="1"/>
-    <col min="20" max="20" width="15.5703125" customWidth="1"/>
-    <col min="21" max="21" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.85546875" customWidth="1"/>
-    <col min="23" max="23" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.7109375" customWidth="1"/>
-    <col min="29" max="29" width="12.5703125" customWidth="1"/>
-    <col min="30" max="30" width="14.85546875" customWidth="1"/>
-    <col min="36" max="36" width="17.42578125" customWidth="1"/>
-    <col min="37" max="37" width="13.7109375" customWidth="1"/>
-    <col min="38" max="38" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="40" max="41" width="12.42578125" customWidth="1"/>
-    <col min="42" max="42" width="23" customWidth="1"/>
-    <col min="43" max="43" width="16.5703125" customWidth="1"/>
-    <col min="44" max="44" width="12" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="18" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="12.28515625" customWidth="1"/>
-    <col min="48" max="48" width="11.42578125" customWidth="1"/>
-    <col min="49" max="49" width="14.28515625" customWidth="1"/>
+    <col min="15" max="15" width="17.42578125" customWidth="1"/>
+    <col min="16" max="16" width="17.7109375" customWidth="1"/>
+    <col min="17" max="17" width="14.5703125" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" customWidth="1"/>
+    <col min="20" max="20" width="25.85546875" customWidth="1"/>
+    <col min="21" max="21" width="15.5703125" customWidth="1"/>
+    <col min="22" max="22" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.85546875" customWidth="1"/>
+    <col min="24" max="24" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.7109375" customWidth="1"/>
+    <col min="30" max="30" width="12.5703125" customWidth="1"/>
+    <col min="31" max="31" width="14.85546875" customWidth="1"/>
+    <col min="37" max="37" width="17.42578125" customWidth="1"/>
+    <col min="38" max="38" width="13.7109375" customWidth="1"/>
+    <col min="39" max="39" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="41" max="42" width="12.42578125" customWidth="1"/>
+    <col min="43" max="43" width="23" customWidth="1"/>
+    <col min="44" max="44" width="16.5703125" customWidth="1"/>
+    <col min="45" max="45" width="12" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="18" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="12.28515625" customWidth="1"/>
+    <col min="49" max="49" width="11.42578125" customWidth="1"/>
+    <col min="50" max="50" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:49">
-      <c r="AL2" s="23"/>
+    <row r="2" spans="1:50">
       <c r="AM2" s="23"/>
-    </row>
-    <row r="3" spans="1:49" s="21" customFormat="1" ht="18.75">
+      <c r="AN2" s="23"/>
+    </row>
+    <row r="3" spans="1:50" s="21" customFormat="1" ht="18.75">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
@@ -1901,55 +1908,56 @@
       <c r="L3" s="61"/>
       <c r="M3" s="61"/>
       <c r="N3" s="61"/>
-      <c r="O3" s="39" t="s">
+      <c r="O3" s="61"/>
+      <c r="P3" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="P3" s="39"/>
       <c r="Q3" s="39"/>
       <c r="R3" s="39"/>
       <c r="S3" s="39"/>
-      <c r="T3" s="16" t="s">
+      <c r="T3" s="39"/>
+      <c r="U3" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="U3" s="16"/>
       <c r="V3" s="16"/>
       <c r="W3" s="16"/>
-      <c r="X3" s="17" t="s">
+      <c r="X3" s="16"/>
+      <c r="Y3" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="Y3" s="17"/>
       <c r="Z3" s="17"/>
       <c r="AA3" s="17"/>
       <c r="AB3" s="17"/>
-      <c r="AC3" s="19" t="s">
+      <c r="AC3" s="17"/>
+      <c r="AD3" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="AD3" s="19"/>
       <c r="AE3" s="19"/>
       <c r="AF3" s="19"/>
       <c r="AG3" s="19"/>
       <c r="AH3" s="19"/>
       <c r="AI3" s="19"/>
-      <c r="AJ3" s="15" t="s">
+      <c r="AJ3" s="19"/>
+      <c r="AK3" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="AK3" s="15"/>
       <c r="AL3" s="15"/>
       <c r="AM3" s="15"/>
       <c r="AN3" s="15"/>
       <c r="AO3" s="15"/>
       <c r="AP3" s="15"/>
-      <c r="AQ3" s="20" t="s">
+      <c r="AQ3" s="15"/>
+      <c r="AR3" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="AR3" s="20"/>
       <c r="AS3" s="20"/>
       <c r="AT3" s="20"/>
       <c r="AU3" s="20"/>
       <c r="AV3" s="20"/>
       <c r="AW3" s="20"/>
-    </row>
-    <row r="4" spans="1:49" s="1" customFormat="1">
+      <c r="AX3" s="20"/>
+    </row>
+    <row r="4" spans="1:50" s="1" customFormat="1">
       <c r="A4" s="11" t="s">
         <v>79</v>
       </c>
@@ -1992,113 +2000,116 @@
       <c r="N4" s="62" t="s">
         <v>270</v>
       </c>
-      <c r="O4" s="40" t="s">
+      <c r="O4" s="62" t="s">
+        <v>271</v>
+      </c>
+      <c r="P4" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="P4" s="40" t="s">
+      <c r="Q4" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="Q4" s="40" t="s">
+      <c r="R4" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="R4" s="40" t="s">
+      <c r="S4" s="40" t="s">
         <v>239</v>
       </c>
-      <c r="S4" s="40" t="s">
+      <c r="T4" s="40" t="s">
         <v>240</v>
       </c>
-      <c r="T4" s="10" t="s">
+      <c r="U4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="U4" s="10" t="s">
+      <c r="V4" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="V4" s="10" t="s">
+      <c r="W4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="W4" s="10" t="s">
+      <c r="X4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="X4" s="9" t="s">
+      <c r="Y4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="Y4" s="9" t="s">
+      <c r="Z4" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="Z4" s="9" t="s">
+      <c r="AA4" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="AA4" s="9" t="s">
+      <c r="AB4" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="AB4" s="9" t="s">
+      <c r="AC4" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="AC4" s="7" t="s">
+      <c r="AD4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="AD4" s="7" t="s">
+      <c r="AE4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="AE4" s="7" t="s">
+      <c r="AF4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="AF4" s="7" t="s">
+      <c r="AG4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="AG4" s="7" t="s">
+      <c r="AH4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="AH4" s="7" t="s">
+      <c r="AI4" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="AI4" s="7" t="s">
+      <c r="AJ4" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="AJ4" s="8" t="s">
+      <c r="AK4" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AK4" s="8" t="s">
+      <c r="AL4" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="AL4" s="8" t="s">
+      <c r="AM4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="AM4" s="8" t="s">
+      <c r="AN4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="AN4" s="8" t="s">
+      <c r="AO4" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="AO4" s="8" t="s">
+      <c r="AP4" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="AP4" s="8" t="s">
+      <c r="AQ4" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="AQ4" s="12" t="s">
+      <c r="AR4" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="AR4" s="12" t="s">
+      <c r="AS4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="AS4" s="12" t="s">
+      <c r="AT4" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="AT4" s="12" t="s">
+      <c r="AU4" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="AU4" s="12" t="s">
+      <c r="AV4" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="AV4" s="12" t="s">
+      <c r="AW4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="AW4" s="12" t="s">
+      <c r="AX4" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:49">
+    <row r="5" spans="1:50">
       <c r="A5" t="s">
         <v>76</v>
       </c>
@@ -2138,115 +2149,118 @@
       <c r="N5">
         <v>0.41860000000000003</v>
       </c>
-      <c r="O5" t="b">
-        <v>0</v>
-      </c>
-      <c r="P5">
+      <c r="O5" t="s">
+        <v>272</v>
+      </c>
+      <c r="P5" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q5">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="T5" t="s">
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="U5" t="s">
         <v>265</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>35</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>20</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>2.75E-2</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
         <v>3</v>
       </c>
-      <c r="Y5">
+      <c r="Z5">
         <v>999</v>
       </c>
-      <c r="Z5">
-        <v>0</v>
-      </c>
-      <c r="AA5" t="s">
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5" t="s">
         <v>251</v>
       </c>
-      <c r="AB5" t="b">
-        <v>0</v>
-      </c>
-      <c r="AC5" t="s">
+      <c r="AC5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD5" t="s">
         <v>112</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
         <v>20</v>
       </c>
-      <c r="AE5">
+      <c r="AF5">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AF5">
+      <c r="AG5">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AG5" s="3">
+      <c r="AH5" s="3">
         <v>0.12</v>
       </c>
-      <c r="AH5" s="5">
+      <c r="AI5" s="5">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AI5" s="38">
+      <c r="AJ5" s="38">
         <v>123</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>31</v>
       </c>
       <c r="AK5" t="s">
         <v>31</v>
       </c>
-      <c r="AL5" s="23">
-        <v>0.88300000000000001</v>
+      <c r="AL5" t="s">
+        <v>31</v>
       </c>
       <c r="AM5" s="23">
         <v>0.88300000000000001</v>
       </c>
-      <c r="AP5" s="43">
-        <v>0</v>
-      </c>
-      <c r="AQ5" t="b">
-        <v>1</v>
+      <c r="AN5" s="23">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="AQ5" s="43">
+        <v>0</v>
       </c>
       <c r="AR5" t="b">
         <v>1</v>
       </c>
       <c r="AS5" t="b">
-        <v>0</v>
-      </c>
-      <c r="AT5">
-        <v>0</v>
-      </c>
-      <c r="AU5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AU5">
+        <v>0</v>
+      </c>
+      <c r="AV5" t="s">
         <v>3</v>
       </c>
-      <c r="AV5" t="b">
-        <v>1</v>
-      </c>
-      <c r="AW5" s="22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:49">
-      <c r="AG6" s="3"/>
-      <c r="AH6" s="5"/>
-      <c r="AI6" s="38"/>
-      <c r="AL6" s="23"/>
+      <c r="AW5" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX5" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:50">
+      <c r="AH6" s="3"/>
+      <c r="AI6" s="5"/>
+      <c r="AJ6" s="38"/>
       <c r="AM6" s="23"/>
-      <c r="AP6" s="43"/>
-      <c r="AW6" s="22"/>
-    </row>
-    <row r="7" spans="1:49">
+      <c r="AN6" s="23"/>
+      <c r="AQ6" s="43"/>
+      <c r="AX6" s="22"/>
+    </row>
+    <row r="7" spans="1:50">
       <c r="B7" s="56" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:49">
+    <row r="8" spans="1:50">
       <c r="A8" t="s">
         <v>248</v>
       </c>
@@ -2277,101 +2291,101 @@
       <c r="J8" t="b">
         <v>0</v>
       </c>
-      <c r="O8" t="b">
-        <v>0</v>
-      </c>
-      <c r="P8">
+      <c r="P8" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q8">
         <v>0.02</v>
       </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="T8" t="s">
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="U8" t="s">
         <v>250</v>
       </c>
-      <c r="U8" t="s">
+      <c r="V8" t="s">
         <v>35</v>
       </c>
-      <c r="V8">
+      <c r="W8">
         <v>20</v>
       </c>
-      <c r="W8">
+      <c r="X8">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="X8">
+      <c r="Y8">
         <v>5</v>
       </c>
-      <c r="Y8">
+      <c r="Z8">
         <v>999</v>
       </c>
-      <c r="Z8">
-        <v>0</v>
-      </c>
-      <c r="AA8" t="s">
+      <c r="AA8">
+        <v>0</v>
+      </c>
+      <c r="AB8" t="s">
         <v>251</v>
       </c>
-      <c r="AB8" t="b">
-        <v>0</v>
-      </c>
-      <c r="AC8" t="s">
+      <c r="AC8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD8" t="s">
         <v>112</v>
       </c>
-      <c r="AD8" t="s">
+      <c r="AE8" t="s">
         <v>20</v>
       </c>
-      <c r="AE8">
+      <c r="AF8">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AF8">
+      <c r="AG8">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AG8" s="3">
+      <c r="AH8" s="3">
         <v>0.12</v>
       </c>
-      <c r="AH8" s="5">
+      <c r="AI8" s="5">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AI8" s="38">
+      <c r="AJ8" s="38">
         <v>123</v>
-      </c>
-      <c r="AJ8" t="s">
-        <v>31</v>
       </c>
       <c r="AK8" t="s">
         <v>31</v>
       </c>
-      <c r="AL8" s="23">
-        <v>0.6976</v>
+      <c r="AL8" t="s">
+        <v>31</v>
       </c>
       <c r="AM8" s="23">
         <v>0.6976</v>
       </c>
-      <c r="AP8" s="43">
+      <c r="AN8" s="23">
+        <v>0.6976</v>
+      </c>
+      <c r="AQ8" s="43">
         <v>0.1</v>
       </c>
-      <c r="AQ8" t="b">
-        <v>1</v>
-      </c>
       <c r="AR8" t="b">
         <v>1</v>
       </c>
       <c r="AS8" t="b">
-        <v>0</v>
-      </c>
-      <c r="AT8">
-        <v>0</v>
-      </c>
-      <c r="AU8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AU8">
+        <v>0</v>
+      </c>
+      <c r="AV8" t="s">
         <v>3</v>
       </c>
-      <c r="AV8" t="b">
-        <v>1</v>
-      </c>
-      <c r="AW8" s="22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:49">
+      <c r="AW8" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX8" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:50">
       <c r="A9" t="s">
         <v>249</v>
       </c>
@@ -2402,109 +2416,109 @@
       <c r="J9" t="b">
         <v>1</v>
       </c>
-      <c r="O9" t="b">
-        <v>0</v>
-      </c>
-      <c r="P9">
+      <c r="P9" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q9">
         <v>0.02</v>
       </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-      <c r="T9" t="s">
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="U9" t="s">
         <v>250</v>
       </c>
-      <c r="U9" t="s">
+      <c r="V9" t="s">
         <v>35</v>
       </c>
-      <c r="V9">
+      <c r="W9">
         <v>20</v>
       </c>
-      <c r="W9">
+      <c r="X9">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="X9">
+      <c r="Y9">
         <v>5</v>
       </c>
-      <c r="Y9">
+      <c r="Z9">
         <v>999</v>
       </c>
-      <c r="Z9">
-        <v>0</v>
-      </c>
-      <c r="AA9" t="s">
+      <c r="AA9">
+        <v>0</v>
+      </c>
+      <c r="AB9" t="s">
         <v>251</v>
       </c>
-      <c r="AB9" t="b">
-        <v>0</v>
-      </c>
-      <c r="AC9" t="s">
+      <c r="AC9" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD9" t="s">
         <v>112</v>
       </c>
-      <c r="AD9" t="s">
+      <c r="AE9" t="s">
         <v>20</v>
       </c>
-      <c r="AE9">
+      <c r="AF9">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AF9">
+      <c r="AG9">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AG9" s="3">
+      <c r="AH9" s="3">
         <v>0.12</v>
       </c>
-      <c r="AH9" s="5">
+      <c r="AI9" s="5">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AI9" s="38">
+      <c r="AJ9" s="38">
         <v>123</v>
       </c>
-      <c r="AJ9" t="s">
+      <c r="AK9" t="s">
         <v>122</v>
       </c>
-      <c r="AK9" t="s">
+      <c r="AL9" t="s">
         <v>123</v>
       </c>
-      <c r="AL9" s="23"/>
       <c r="AM9" s="23"/>
-      <c r="AN9" s="44">
-        <v>81825573157</v>
-      </c>
+      <c r="AN9" s="23"/>
       <c r="AO9" s="44">
         <v>81825573157</v>
       </c>
-      <c r="AP9" s="43">
+      <c r="AP9" s="44">
+        <v>81825573157</v>
+      </c>
+      <c r="AQ9" s="43">
         <v>0.1</v>
       </c>
-      <c r="AQ9" t="b">
-        <v>1</v>
-      </c>
       <c r="AR9" t="b">
         <v>1</v>
       </c>
       <c r="AS9" t="b">
-        <v>0</v>
-      </c>
-      <c r="AT9">
-        <v>0</v>
-      </c>
-      <c r="AU9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT9" t="b">
+        <v>0</v>
+      </c>
+      <c r="AU9">
+        <v>0</v>
+      </c>
+      <c r="AV9" t="s">
         <v>3</v>
       </c>
-      <c r="AV9" t="b">
-        <v>1</v>
-      </c>
-      <c r="AW9" s="22" t="b">
+      <c r="AW9" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX9" s="22" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="15" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR5:AS6 C5:C6 C8:C9 AR8:AS9" xr:uid="{1240F49A-5091-456D-B77A-0673AD56E758}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS5:AT6 C5:C6 C8:C9 AS8:AT9" xr:uid="{1240F49A-5091-456D-B77A-0673AD56E758}">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC5:AC6 AC8:AC9" xr:uid="{8909875A-86FC-4594-BBAF-A364A5851F3C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD5:AD6 AD8:AD9" xr:uid="{8909875A-86FC-4594-BBAF-A364A5851F3C}">
       <formula1>"simple, internal"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D6 D8:D9" xr:uid="{EC327A6A-3FD9-4228-86E6-BF4DFCBDFAEB}">

</xml_diff>

<commit_message>
corret asset smoothing parameter
</commit_message>
<xml_diff>
--- a/model/RunControl.xlsx
+++ b/model/RunControl.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550597FF-EA2F-493E-A8A1-33E52445F57A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880F0B0D-FB56-4916-840E-48BE4824945F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1845" windowWidth="29040" windowHeight="15840" tabRatio="524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -235,7 +235,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="276">
   <si>
     <t>nsim</t>
   </si>
@@ -1124,6 +1124,9 @@
   <si>
     <t>sharedNC and fixed COLA, EEC can be 0</t>
   </si>
+  <si>
+    <t>method1</t>
+  </si>
 </sst>
 </file>
 
@@ -1139,7 +1142,7 @@
     <numFmt numFmtId="168" formatCode="0.000%"/>
     <numFmt numFmtId="169" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1249,12 +1252,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="14">
@@ -1477,11 +1474,11 @@
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1502,10 +1499,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1849,10 +1842,10 @@
   <dimension ref="A2:BC11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="M5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="Z5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="U20" sqref="U20"/>
+      <selection pane="bottomRight" activeCell="AH16" sqref="AH16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2006,7 +1999,7 @@
       <c r="J4" s="45" t="s">
         <v>115</v>
       </c>
-      <c r="K4" s="63" t="s">
+      <c r="K4" s="62" t="s">
         <v>251</v>
       </c>
       <c r="L4" s="60" t="s">
@@ -2036,7 +2029,7 @@
       <c r="T4" s="60" t="s">
         <v>260</v>
       </c>
-      <c r="U4" s="63" t="s">
+      <c r="U4" s="62" t="s">
         <v>254</v>
       </c>
       <c r="V4" s="60" t="s">
@@ -2138,7 +2131,7 @@
       <c r="BB4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="BC4" s="64" t="s">
+      <c r="BC4" s="63" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2231,7 +2224,7 @@
         <v>0</v>
       </c>
       <c r="AG5" t="s">
-        <v>231</v>
+        <v>275</v>
       </c>
       <c r="AH5" t="b">
         <v>0</v>
@@ -2701,7 +2694,7 @@
         <v>0</v>
       </c>
       <c r="AG9" t="s">
-        <v>231</v>
+        <v>275</v>
       </c>
       <c r="AH9" t="b">
         <v>0</v>
@@ -2862,7 +2855,7 @@
         <v>0</v>
       </c>
       <c r="AG10" t="s">
-        <v>231</v>
+        <v>275</v>
       </c>
       <c r="AH10" t="b">
         <v>0</v>
@@ -3023,7 +3016,7 @@
         <v>0</v>
       </c>
       <c r="AG11" t="s">
-        <v>231</v>
+        <v>275</v>
       </c>
       <c r="AH11" t="b">
         <v>0</v>
@@ -5012,7 +5005,7 @@
         <v>-0.24</v>
       </c>
       <c r="F6" s="6">
-        <f t="shared" ref="F4:F6" si="4">B6 - C6^2/2</f>
+        <f t="shared" ref="F6" si="4">B6 - C6^2/2</f>
         <v>-0.24</v>
       </c>
     </row>
@@ -6154,15 +6147,15 @@
       </c>
     </row>
     <row r="3" spans="1:18">
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="64" t="s">
         <v>204</v>
       </c>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62" t="s">
+      <c r="C3" s="64"/>
+      <c r="D3" s="64" t="s">
         <v>205</v>
       </c>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="1"/>

</xml_diff>